<commit_message>
Se libera nueva version sin numero.
</commit_message>
<xml_diff>
--- a/Programas/estructura paso.xlsx
+++ b/Programas/estructura paso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Paso</t>
   </si>
@@ -42,96 +42,9 @@
     <t>F</t>
   </si>
   <si>
-    <t>DW110</t>
-  </si>
-  <si>
-    <t>DW120</t>
-  </si>
-  <si>
-    <t>ROTA</t>
-  </si>
-  <si>
-    <t>DW130</t>
-  </si>
-  <si>
-    <t>DW140</t>
-  </si>
-  <si>
-    <t>DW160</t>
-  </si>
-  <si>
-    <t>DW170</t>
-  </si>
-  <si>
-    <t>DW180</t>
-  </si>
-  <si>
-    <t>DW190</t>
-  </si>
-  <si>
-    <t>MANT</t>
-  </si>
-  <si>
-    <t>TEMP</t>
-  </si>
-  <si>
-    <t>FIN</t>
-  </si>
-  <si>
-    <t>Dir</t>
-  </si>
-  <si>
-    <t>Texto</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Plantilla</t>
-  </si>
-  <si>
     <t>FUNCION</t>
   </si>
   <si>
-    <t>h414D</t>
-  </si>
-  <si>
-    <t>h4554</t>
-  </si>
-  <si>
-    <t>h4946</t>
-  </si>
-  <si>
-    <t>h554D</t>
-  </si>
-  <si>
-    <t>h4441</t>
-  </si>
-  <si>
-    <t>h4544</t>
-  </si>
-  <si>
-    <t>h4C4C</t>
-  </si>
-  <si>
-    <t>h4F52</t>
-  </si>
-  <si>
-    <t>h4543</t>
-  </si>
-  <si>
-    <t>DW100</t>
-  </si>
-  <si>
-    <t>FUNC</t>
-  </si>
-  <si>
-    <t>Dec</t>
-  </si>
-  <si>
-    <t>DW150</t>
-  </si>
-  <si>
     <t>NUMERO</t>
   </si>
   <si>
@@ -141,15 +54,6 @@
     <t>ARGS</t>
   </si>
   <si>
-    <t>ALGO</t>
-  </si>
-  <si>
-    <t>TRAB</t>
-  </si>
-  <si>
-    <t>ENFR</t>
-  </si>
-  <si>
     <t>TEMPSALIDA</t>
   </si>
   <si>
@@ -187,6 +91,9 @@
   </si>
   <si>
     <t>TempSalida</t>
+  </si>
+  <si>
+    <t>PasoGrafica</t>
   </si>
 </sst>
 </file>
@@ -264,17 +171,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,7 +558,7 @@
   <dimension ref="A2:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -660,18 +567,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
@@ -707,7 +614,7 @@
     </row>
     <row r="4" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
@@ -724,7 +631,7 @@
     </row>
     <row r="5" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
@@ -743,7 +650,7 @@
     </row>
     <row r="6" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
@@ -755,39 +662,39 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
@@ -795,12 +702,14 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -808,7 +717,7 @@
     </row>
     <row r="9" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
@@ -818,10 +727,10 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -853,10 +762,10 @@
     </row>
     <row r="12" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -864,13 +773,13 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -898,306 +807,199 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>0</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="1"/>
-      <c r="H16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="1"/>
-      <c r="H17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="2" t="str">
-        <f>"h" &amp; DEC2HEX(CODE(MID(I17,2,1))) &amp; DEC2HEX(CODE(MID(I17,1,1)))</f>
-        <v>h5546</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" ref="K17:K20" si="0">HEX2DEC(SUBSTITUTE(J17,"h",""))</f>
-        <v>21830</v>
-      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>2</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="1"/>
-      <c r="H18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" si="0"/>
-        <v>17731</v>
-      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>3</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="1"/>
-      <c r="H19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" si="0"/>
-        <v>20306</v>
-      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>4</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="1"/>
-      <c r="H20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K20" s="5">
-        <f t="shared" si="0"/>
-        <v>19532</v>
-      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>5</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="1"/>
-      <c r="H21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" s="5">
-        <f>HEX2DEC(SUBSTITUTE(J21,"h",""))</f>
-        <v>17732</v>
-      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>6</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="1"/>
-      <c r="H22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22" s="5">
-        <f t="shared" ref="K22:K28" si="1">HEX2DEC(SUBSTITUTE(J22,"h",""))</f>
-        <v>17473</v>
-      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>7</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="1"/>
-      <c r="H23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="5">
-        <f t="shared" si="1"/>
-        <v>21837</v>
-      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>8</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="1"/>
-      <c r="H24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K24" s="5">
-        <f t="shared" si="1"/>
-        <v>18758</v>
-      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="5"/>
     </row>
     <row r="25" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>9</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="5">
-        <f t="shared" si="1"/>
-        <v>17748</v>
-      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K26" s="5">
-        <f t="shared" si="1"/>
-        <v>16717</v>
-      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="5"/>
     </row>
     <row r="27" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="2"/>
       <c r="I27" s="6"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K27" s="5"/>
     </row>
     <row r="28" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="2"/>
       <c r="I28" s="6"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K28" s="5"/>
     </row>
     <row r="29" spans="2:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1209,9 +1011,9 @@
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1223,9 +1025,9 @@
       <c r="B31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1235,11 +1037,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="H15:K15"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
@@ -1248,12 +1051,11 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>
@@ -1279,7 +1081,7 @@
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Se libera version 1.03 de PLC y 1.03 de HMI. * Se implementa #1, memoria en caso de perdida de energia. * Se corrige #13, P09 (vacio ventilador principal) no incluido en la seguridades. * Se corrige #14, P0A (vacio ventilador de quemador) no incluido en las seguridades.
</commit_message>
<xml_diff>
--- a/Programas/estructura paso.xlsx
+++ b/Programas/estructura paso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Paso</t>
   </si>
@@ -108,7 +108,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +125,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -155,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -171,16 +177,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -558,7 +567,7 @@
   <dimension ref="A2:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -567,30 +576,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2">
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="11">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="11">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="11">
         <v>3</v>
       </c>
       <c r="F3" s="2">
@@ -616,12 +625,12 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -633,12 +642,12 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11">
         <v>2</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -652,12 +661,12 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11">
         <v>3</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -673,35 +682,37 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="2" t="s">
         <v>25</v>
       </c>
@@ -719,12 +730,12 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
         <v>20</v>
@@ -737,10 +748,10 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -749,10 +760,10 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -761,14 +772,14 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -807,26 +818,26 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>0</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
       <c r="F16" s="1"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -837,9 +848,9 @@
       <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="1"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -850,9 +861,9 @@
       <c r="B18" s="2">
         <v>2</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="1"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -863,9 +874,9 @@
       <c r="B19" s="2">
         <v>3</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="1"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -876,9 +887,9 @@
       <c r="B20" s="2">
         <v>4</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
       <c r="F20" s="1"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -889,9 +900,9 @@
       <c r="B21" s="2">
         <v>5</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="1"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -902,9 +913,9 @@
       <c r="B22" s="2">
         <v>6</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="1"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -915,9 +926,9 @@
       <c r="B23" s="2">
         <v>7</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="1"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -928,9 +939,9 @@
       <c r="B24" s="2">
         <v>8</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="1"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -941,9 +952,9 @@
       <c r="B25" s="2">
         <v>9</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="2"/>
@@ -955,9 +966,9 @@
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="2"/>
@@ -969,9 +980,9 @@
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="2"/>
@@ -983,9 +994,9 @@
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="2"/>
@@ -997,9 +1008,9 @@
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1011,9 +1022,9 @@
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1025,9 +1036,9 @@
       <c r="B31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1037,12 +1048,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
@@ -1051,11 +1061,12 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="H15:K15"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>